<commit_message>
Closed #130 Sfera assegna colore
</commit_message>
<xml_diff>
--- a/docs/tp/Sfera_4.0/TP NR ALLIANZ.xlsx
+++ b/docs/tp/Sfera_4.0/TP NR ALLIANZ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TA\matrix-web-fe-tests\docs\tp\Sfera_4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386D0DF7-C758-4F37-8E0F-F345AA5D17BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD542F12-8A55-4D4A-B43A-978D000E1693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="84">
   <si>
     <t>Titolo</t>
   </si>
@@ -274,6 +274,12 @@
   </si>
   <si>
     <t>DA FARE</t>
+  </si>
+  <si>
+    <t>INSERITO IN GIT PROJECT</t>
+  </si>
+  <si>
+    <t>INSERITO IN GIT PROJECT (no check mail)</t>
   </si>
 </sst>
 </file>
@@ -686,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1488"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -734,9 +740,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="4" customFormat="1" ht="38.25">
+    <row r="2" spans="1:10" s="4" customFormat="1" ht="25.5">
       <c r="A2" s="9" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>9</v>
@@ -777,9 +783,9 @@
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
     </row>
-    <row r="4" spans="1:10" s="4" customFormat="1" ht="38.25">
+    <row r="4" spans="1:10" s="4" customFormat="1" ht="25.5">
       <c r="A4" s="9" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>17</v>
@@ -848,7 +854,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="11" customFormat="1" ht="89.25">
+    <row r="7" spans="1:10" s="11" customFormat="1" ht="102">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10" t="s">
@@ -908,7 +914,7 @@
     </row>
     <row r="10" spans="1:10" s="4" customFormat="1" ht="25.5">
       <c r="A10" s="9" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>20</v>
@@ -949,9 +955,9 @@
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
     </row>
-    <row r="12" spans="1:10" s="4" customFormat="1" ht="25.5">
+    <row r="12" spans="1:10" s="4" customFormat="1" ht="38.25">
       <c r="A12" s="9" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>22</v>
@@ -994,7 +1000,7 @@
     </row>
     <row r="14" spans="1:10" s="11" customFormat="1" ht="25.5">
       <c r="A14" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>23</v>
@@ -1037,7 +1043,7 @@
     </row>
     <row r="16" spans="1:10" s="4" customFormat="1" ht="25.5">
       <c r="A16" s="9" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>24</v>
@@ -1080,7 +1086,7 @@
     </row>
     <row r="18" spans="1:10" s="11" customFormat="1" ht="25.5">
       <c r="A18" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>26</v>
@@ -1123,7 +1129,7 @@
     </row>
     <row r="20" spans="1:10" s="11" customFormat="1" ht="25.5">
       <c r="A20" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>28</v>
@@ -1192,7 +1198,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="11" customFormat="1" ht="89.25">
+    <row r="23" spans="1:10" s="11" customFormat="1" ht="102">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10" t="s">
@@ -1347,7 +1353,7 @@
       <c r="H30" s="10"/>
       <c r="I30" s="10"/>
     </row>
-    <row r="31" spans="1:10" s="13" customFormat="1" ht="51">
+    <row r="31" spans="1:10" s="13" customFormat="1" ht="38.25">
       <c r="A31" s="12" t="s">
         <v>75</v>
       </c>
@@ -1418,7 +1424,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="4" customFormat="1" ht="127.5">
+    <row r="34" spans="1:10" s="4" customFormat="1" ht="140.25">
       <c r="A34" s="9"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9" t="s">
@@ -1564,7 +1570,7 @@
       <c r="H41" s="9"/>
       <c r="I41" s="9"/>
     </row>
-    <row r="42" spans="1:10" s="13" customFormat="1" ht="102">
+    <row r="42" spans="1:10" s="13" customFormat="1" ht="76.5">
       <c r="A42" s="12" t="s">
         <v>76</v>
       </c>
@@ -1607,7 +1613,7 @@
       <c r="H43" s="12"/>
       <c r="I43" s="12"/>
     </row>
-    <row r="44" spans="1:10" s="13" customFormat="1" ht="102">
+    <row r="44" spans="1:10" s="13" customFormat="1" ht="76.5">
       <c r="A44" s="12" t="s">
         <v>76</v>
       </c>
@@ -1693,7 +1699,7 @@
       <c r="H47" s="10"/>
       <c r="I47" s="10"/>
     </row>
-    <row r="48" spans="1:10" s="13" customFormat="1" ht="102">
+    <row r="48" spans="1:10" s="13" customFormat="1" ht="76.5">
       <c r="A48" s="12" t="s">
         <v>76</v>
       </c>

</xml_diff>

<commit_message>
Aggiornato TP Sfera 4.0 AZ
</commit_message>
<xml_diff>
--- a/docs/tp/Sfera_4.0/TP NR ALLIANZ.xlsx
+++ b/docs/tp/Sfera_4.0/TP NR ALLIANZ.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TA\matrix-web-fe-tests\docs\tp\Sfera_4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD542F12-8A55-4D4A-B43A-978D000E1693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D91741-5B17-42C0-B3A4-A3FC33AF87AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="84">
   <si>
     <t>Titolo</t>
   </si>
@@ -692,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1488"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1172,7 +1172,7 @@
     </row>
     <row r="22" spans="1:10" s="11" customFormat="1" ht="25.5">
       <c r="A22" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>31</v>
@@ -1215,7 +1215,7 @@
     </row>
     <row r="24" spans="1:10" s="11" customFormat="1" ht="38.25">
       <c r="A24" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>32</v>
@@ -1270,7 +1270,9 @@
       <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:10" s="11" customFormat="1" ht="25.5">
-      <c r="A27" s="10"/>
+      <c r="A27" s="10" t="s">
+        <v>81</v>
+      </c>
       <c r="B27" s="10" t="s">
         <v>35</v>
       </c>
@@ -1658,7 +1660,7 @@
     </row>
     <row r="46" spans="1:10" s="11" customFormat="1" ht="25.5">
       <c r="A46" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B46" s="10" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
Aggiornamento BRAIN Aprile 22 AZ
</commit_message>
<xml_diff>
--- a/docs/tp/Sfera_4.0/TP NR ALLIANZ.xlsx
+++ b/docs/tp/Sfera_4.0/TP NR ALLIANZ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TA\matrix-web-fe-tests\docs\tp\Sfera_4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99571FA9-EA17-416E-9B58-7056243B043C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E441AD-F973-43C4-9F3A-144CA070223A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -692,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1488"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1314,7 +1314,7 @@
     </row>
     <row r="29" spans="1:10" s="11" customFormat="1" ht="25.5">
       <c r="A29" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>36</v>

</xml_diff>